<commit_message>
comparison methods - final
</commit_message>
<xml_diff>
--- a/datasets/Example.xlsx
+++ b/datasets/Example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OWD\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B294721-0B34-4CF3-9253-7934C40F681C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08870E5F-8F52-4174-AAE1-D38792825DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19080" windowHeight="15585" activeTab="1" xr2:uid="{179F6171-9608-4223-8501-83E61A659394}"/>
+    <workbookView xWindow="1455" yWindow="3225" windowWidth="19755" windowHeight="15345" xr2:uid="{179F6171-9608-4223-8501-83E61A659394}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,9 +63,6 @@
     <t>A1</t>
   </si>
   <si>
-    <t>A2</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
@@ -73,6 +70,9 @@
   </si>
   <si>
     <t>z</t>
+  </si>
+  <si>
+    <t>A0</t>
   </si>
 </sst>
 </file>
@@ -434,8 +434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5874DD41-4C42-4CBE-99E0-F84EC7FBE12E}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,13 +455,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>10</v>
-      </c>
-      <c r="E1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -472,13 +472,13 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0.34</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -489,13 +489,13 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>0.316</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>7.7</v>
       </c>
       <c r="E3">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -506,13 +506,13 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>0.60799999999999998</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>7.8</v>
       </c>
       <c r="E4">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -523,13 +523,13 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>0.3</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>7.9</v>
       </c>
       <c r="E5">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -542,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B3019DB-86FC-49F3-AA91-A5CA8D151DF8}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,13 +556,13 @@
         <v>6</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -570,27 +570,27 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>7.6</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>0.7</v>
+      </c>
+      <c r="C3">
         <v>8</v>
       </c>
-      <c r="B3">
-        <v>9</v>
-      </c>
-      <c r="C3">
-        <v>9</v>
-      </c>
       <c r="D3">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>